<commit_message>
fixed air infiltration calculation
</commit_message>
<xml_diff>
--- a/heat_loss_estimates.xlsx
+++ b/heat_loss_estimates.xlsx
@@ -5,16 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="house" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="garage" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ICF house" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="BTU_per_wh" vbProcedure="false">garage!$N$5</definedName>
     <definedName function="false" hidden="false" name="M2_per_sqft" vbProcedure="false">garage!$N$2</definedName>
     <definedName function="false" hidden="false" name="RSI_per_R" vbProcedure="false">garage!$N$3</definedName>
+    <definedName function="false" hidden="false" name="watthour_to_MJ" vbProcedure="false">house!$G$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t xml:space="preserve">https://www.engineeringtoolbox.com/heat-loss-transmission-d_748.html</t>
   </si>
@@ -37,7 +39,7 @@
     <t xml:space="preserve">outside temperature C</t>
   </si>
   <si>
-    <t xml:space="preserve">desired inside temperature C</t>
+    <t xml:space="preserve">req’d inside temperature C</t>
   </si>
   <si>
     <t xml:space="preserve">heating power (W)</t>
@@ -53,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watt-hour to MJ</t>
   </si>
   <si>
     <t xml:space="preserve">1 year</t>
@@ -154,13 +159,22 @@
     <t xml:space="preserve">Floor back cantilever</t>
   </si>
   <si>
+    <t xml:space="preserve">air infiltration</t>
+  </si>
+  <si>
     <t xml:space="preserve">leaks</t>
   </si>
   <si>
-    <t xml:space="preserve">volume </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cubic meters</t>
+    <t xml:space="preserve">volume of house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3 – back calculated from EqLA and ACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H i = Cp ρ n V (t i - t o )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.engineeringtoolbox.com/heat-loss-buildings-d_113.html</t>
   </si>
   <si>
     <t xml:space="preserve">air changes per hour</t>
@@ -169,7 +183,10 @@
     <t xml:space="preserve">measured 1.75 at 50 Pa</t>
   </si>
   <si>
-    <t xml:space="preserve">infiltration loss is in Imperial, convert to metric for MJ output</t>
+    <t xml:space="preserve">Cp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kJ/kgK </t>
   </si>
   <si>
     <t xml:space="preserve">equivalent leak area (EqLA)</t>
@@ -178,7 +195,10 @@
     <t xml:space="preserve">cm^2</t>
   </si>
   <si>
-    <t xml:space="preserve">0.018*BTU/h_to_W*C_to_degreeF*m3toCF</t>
+    <t xml:space="preserve">ρ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/m3</t>
   </si>
   <si>
     <t xml:space="preserve">cfm50</t>
@@ -187,10 +207,13 @@
     <t xml:space="preserve">cubic feet per minute</t>
   </si>
   <si>
+    <t xml:space="preserve">hours/second</t>
+  </si>
+  <si>
     <t xml:space="preserve">∆T</t>
   </si>
   <si>
-    <t xml:space="preserve">rate of heat loss (W)</t>
+    <t xml:space="preserve">rate of heat loss (watts)</t>
   </si>
   <si>
     <t xml:space="preserve">desired temperature</t>
@@ -221,63 +244,121 @@
   </si>
   <si>
     <t xml:space="preserve">R-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design
+ΔT
+°C or K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy
+transfer
+MJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13 walls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ceiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7.5 wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assuming 26’x20’ footprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desired inside temperature C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">windows avg U-factor</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Design
-ΔT
-</t>
+      <t xml:space="preserve">Floor header 1</t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <vertAlign val="superscript"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">°C or K</t>
+      <t xml:space="preserve">st</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy
-transfer
-MJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R13 walls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ceiling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7.5 wall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assuming 26’x20’ footprint</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> floor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Floor header 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> floor</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Basement-1 pony wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basement-1 header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volume </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cubic meters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -305,6 +386,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -316,11 +408,10 @@
       <family val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -371,13 +462,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -412,8 +507,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -421,6 +524,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,7 +745,7 @@
             <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Rate of heat loss (W/K) = V x ACH x ∆T x 0.33 </a:t>
+            <a:t>Rate of heat loss (W/K) = V x ACH x ∆T x Kfactor </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -654,7 +761,7 @@
             <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>ACH – air changes per hour </a:t>
+            <a:t>ACH – air changes per hour</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -670,7 +777,13 @@
             <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Rate of heat loss per ˚C difference between inside and outside = V x ACH x 0.33</a:t>
+            <a:t>Rate of heat loss per ˚C difference between inside </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>and outside = V x ACH x Kfactor</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -686,7 +799,7 @@
             <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>0.33 product of specific heat capacity and density of air </a:t>
+            <a:t>Kfactor make the units work out</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -702,7 +815,7 @@
             <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>V is the volume of the room</a:t>
+            <a:t>V is the volume of the room in cubic meters</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -724,7 +837,7 @@
             <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>T is the temperature difference</a:t>
+            <a:t>T is the temperature difference in degrees C</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -760,6 +873,115 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3982680" y="239760"/>
+          <a:ext cx="3508560" cy="1348200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Φ = A × U × ΔT</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>where Φ is the heat transfer in watts, </a:t>
+          </a:r>
+          <a:br/>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>U is the thermal transmittance, </a:t>
+          </a:r>
+          <a:br/>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>ΔT is the temperature differential across the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>structure, </a:t>
+          </a:r>
+          <a:br/>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>A is the area in square metres.</a:t>
+          </a:r>
+          <a:br/>
+          <a:br/>
+          <a:r>
+            <a:rPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+              <a:hlinkClick r:id="rId1"/>
+            </a:rPr>
+            <a:t>https://en.wikipedia.org/wiki/Thermal_transmittance</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr b="0" lang="en-CA" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>312120</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>96480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>743040</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>144360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextShape 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4262400" y="96480"/>
           <a:ext cx="3508560" cy="1348200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -845,10 +1067,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -875,32 +1097,32 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>-10</v>
+      <c r="B4" s="2" t="n">
+        <v>6.2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>20</v>
+      <c r="B5" s="2" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <f aca="false">SUM(H16:H29)</f>
-        <v>7819.93536574475</v>
+      <c r="B7" s="4" t="n">
+        <f aca="false">SUM(H16:H30)</f>
+        <v>2881.1659005976</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -912,683 +1134,699 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="5" t="n">
         <f aca="false">24*C9/C11</f>
         <v>9.85626283367557</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">24*365.25</f>
         <v>8766</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <f aca="false">SUM(I16:I29)/1000</f>
-        <v>81.0770898720416</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <f aca="false">SUM(I16:I30)/1000</f>
+        <v>90.9226810246987</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
       <c r="O12" s="0" t="n">
         <f aca="false">2*1.2+0.5*PI()*1.2</f>
         <v>4.28495559215388</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="5" t="n">
         <f aca="false">1000*C12/C9</f>
-        <v>22.5214138533449</v>
+        <v>25.2563002846385</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="3"/>
-      <c r="I14" s="4"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="I15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="J15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C16" s="4" t="n">
+      <c r="C16" s="5" t="n">
         <f aca="false">1/D16</f>
         <v>0.357142857142857</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="8" t="n">
         <v>2.8</v>
       </c>
-      <c r="E16" s="8" t="n">
+      <c r="E16" s="9" t="n">
         <v>25.45</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <f aca="false">D16*E16</f>
         <v>71.26</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H16" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H16" s="4" t="n">
         <f aca="false">F16*G16</f>
-        <v>2137.8</v>
-      </c>
-      <c r="I16" s="3" t="n">
-        <f aca="false">F16*$C$11*0.0036*$C$10</f>
-        <v>22164.7104</v>
-      </c>
-      <c r="J16" s="9" t="n">
+        <v>840.868</v>
+      </c>
+      <c r="I16" s="4" t="n">
+        <f aca="false">F16*G16*$C$11*watthour_to_MJ</f>
+        <v>26535.7759968</v>
+      </c>
+      <c r="J16" s="10" t="n">
         <f aca="false">I16/($C$12*1000)</f>
-        <v>0.273378218618614</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+        <v>0.291849906951068</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="7" t="n">
-        <v>2.39</v>
-      </c>
-      <c r="D17" s="4" t="n">
+      <c r="C17" s="8" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="D17" s="5" t="n">
         <f aca="false">1/C17</f>
-        <v>0.418410041841004</v>
-      </c>
-      <c r="E17" s="8" t="n">
+        <v>0.280898876404494</v>
+      </c>
+      <c r="E17" s="9" t="n">
         <v>122</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <f aca="false">D17*E17</f>
-        <v>51.0460251046025</v>
+        <v>34.2696629213483</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H17" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H17" s="4" t="n">
         <f aca="false">F17*G17</f>
-        <v>1531.38075313808</v>
-      </c>
-      <c r="I17" s="3" t="n">
-        <f aca="false">F17*$C$11*0.0036*$C$10</f>
-        <v>15877.3556485356</v>
-      </c>
-      <c r="J17" s="9" t="n">
+        <v>404.38202247191</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <f aca="false">F17*G17*$C$11*watthour_to_MJ</f>
+        <v>12761.3261123596</v>
+      </c>
+      <c r="J17" s="10" t="n">
         <f aca="false">I17/($C$12*1000)</f>
-        <v>0.19583035939738</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+        <v>0.140353605596969</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="8" t="n">
         <v>3.56</v>
       </c>
-      <c r="D18" s="4" t="n">
+      <c r="D18" s="5" t="n">
         <f aca="false">1/C18</f>
         <v>0.280898876404494</v>
       </c>
-      <c r="E18" s="8" t="n">
+      <c r="E18" s="9" t="n">
         <v>102.9</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="5" t="n">
         <f aca="false">D18*E18</f>
         <v>28.9044943820225</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H18" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H18" s="4" t="n">
         <f aca="false">F18*G18</f>
-        <v>867.134831460674</v>
-      </c>
-      <c r="I18" s="3" t="n">
-        <f aca="false">F18*$C$11*0.0036*$C$10</f>
-        <v>8990.45393258427</v>
-      </c>
-      <c r="J18" s="9" t="n">
+        <v>341.073033707865</v>
+      </c>
+      <c r="I18" s="4" t="n">
+        <f aca="false">F18*G18*$C$11*watthour_to_MJ</f>
+        <v>10763.4463685393</v>
+      </c>
+      <c r="J18" s="10" t="n">
         <f aca="false">I18/($C$12*1000)</f>
-        <v>0.110887723606919</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+        <v>0.118380213245312</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C19" s="4" t="n">
+      <c r="C19" s="5" t="n">
         <f aca="false">1/D19</f>
         <v>0.384615384615385</v>
       </c>
-      <c r="D19" s="7" t="n">
+      <c r="D19" s="8" t="n">
         <v>2.6</v>
       </c>
-      <c r="E19" s="8" t="n">
+      <c r="E19" s="9" t="n">
         <v>9.86</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="5" t="n">
         <f aca="false">D19*E19</f>
         <v>25.636</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H19" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H19" s="4" t="n">
         <f aca="false">F19*G19</f>
-        <v>769.08</v>
-      </c>
-      <c r="I19" s="3" t="n">
-        <f aca="false">F19*$C$11*0.0036*$C$10</f>
-        <v>7973.82144</v>
-      </c>
-      <c r="J19" s="9" t="n">
+        <v>302.5048</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <f aca="false">F19*G19*$C$11*watthour_to_MJ</f>
+        <v>9546.32547648</v>
+      </c>
+      <c r="J19" s="10" t="n">
         <f aca="false">I19/($C$12*1000)</f>
-        <v>0.0983486389630478</v>
-      </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+        <v>0.104993884571956</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="8" t="n">
         <v>8.54</v>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="5" t="n">
         <f aca="false">1/C20</f>
         <v>0.117096018735363</v>
       </c>
-      <c r="E20" s="8" t="n">
+      <c r="E20" s="9" t="n">
         <v>160.3</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <f aca="false">D20*E20</f>
         <v>18.7704918032787</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H20" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H20" s="4" t="n">
         <f aca="false">F20*G20</f>
-        <v>563.114754098361</v>
-      </c>
-      <c r="I20" s="3" t="n">
-        <f aca="false">F20*$C$11*0.0036*$C$10</f>
-        <v>5838.37377049181</v>
-      </c>
-      <c r="J20" s="9" t="n">
+        <v>221.491803278689</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <f aca="false">F20*G20*$C$11*watthour_to_MJ</f>
+        <v>6989.74973114754</v>
+      </c>
+      <c r="J20" s="10" t="n">
         <f aca="false">I20/($C$12*1000)</f>
-        <v>0.0720101545295485</v>
-      </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+        <v>0.0768757547882779</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="8" t="n">
         <v>2.7</v>
       </c>
-      <c r="D21" s="4" t="n">
+      <c r="D21" s="5" t="n">
         <f aca="false">1/C21</f>
         <v>0.37037037037037</v>
       </c>
-      <c r="E21" s="8" t="n">
+      <c r="E21" s="9" t="n">
         <v>40.9</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="5" t="n">
         <f aca="false">D21*E21</f>
         <v>15.1481481481481</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H21" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H21" s="4" t="n">
         <f aca="false">F21*G21</f>
-        <v>454.444444444444</v>
-      </c>
-      <c r="I21" s="3" t="n">
-        <f aca="false">F21*$C$11*0.0036*$C$10</f>
-        <v>4711.68</v>
-      </c>
-      <c r="J21" s="9" t="n">
+        <v>178.748148148148</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <f aca="false">F21*G21*$C$11*watthour_to_MJ</f>
+        <v>5640.86256</v>
+      </c>
+      <c r="J21" s="10" t="n">
         <f aca="false">I21/($C$12*1000)</f>
-        <v>0.058113580635863</v>
-      </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+        <v>0.0620402136895599</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="8" t="n">
         <v>2.78</v>
       </c>
-      <c r="D22" s="4" t="n">
+      <c r="D22" s="5" t="n">
         <f aca="false">1/C22</f>
         <v>0.359712230215827</v>
       </c>
-      <c r="E22" s="8" t="n">
+      <c r="E22" s="9" t="n">
         <v>33.4</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <f aca="false">D22*E22</f>
         <v>12.0143884892086</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H22" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H22" s="4" t="n">
         <f aca="false">F22*G22</f>
-        <v>360.431654676259</v>
-      </c>
-      <c r="I22" s="3" t="n">
-        <f aca="false">F22*$C$11*0.0036*$C$10</f>
-        <v>3736.95539568345</v>
-      </c>
-      <c r="J22" s="9" t="n">
+        <v>141.769784172662</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <f aca="false">F22*G22*$C$11*watthour_to_MJ</f>
+        <v>4473.9141410072</v>
+      </c>
+      <c r="J22" s="10" t="n">
         <f aca="false">I22/($C$12*1000)</f>
-        <v>0.0460913853911288</v>
-      </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+        <v>0.0492056997284525</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="8" t="n">
         <v>1.77</v>
       </c>
-      <c r="D23" s="4" t="n">
+      <c r="D23" s="5" t="n">
         <f aca="false">1/C23</f>
         <v>0.564971751412429</v>
       </c>
-      <c r="E23" s="8" t="n">
+      <c r="E23" s="9" t="n">
         <v>19.7</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="5" t="n">
         <f aca="false">D23*E23</f>
         <v>11.1299435028249</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H23" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H23" s="4" t="n">
         <f aca="false">F23*G23</f>
-        <v>333.898305084746</v>
-      </c>
-      <c r="I23" s="3" t="n">
-        <f aca="false">F23*$C$11*0.0036*$C$10</f>
-        <v>3461.85762711864</v>
-      </c>
-      <c r="J23" s="9" t="n">
+        <v>131.333333333333</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <f aca="false">F23*G23*$C$11*watthour_to_MJ</f>
+        <v>4144.5648</v>
+      </c>
+      <c r="J23" s="10" t="n">
         <f aca="false">I23/($C$12*1000)</f>
-        <v>0.0426983458900937</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+        <v>0.0455833984797935</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="5" t="n">
         <f aca="false">1/D24</f>
         <v>10</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="8" t="n">
         <v>0.1</v>
       </c>
-      <c r="E24" s="8" t="n">
+      <c r="E24" s="9" t="n">
         <v>64.8</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="5" t="n">
         <f aca="false">D24*E24</f>
         <v>6.48</v>
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H24" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H24" s="4" t="n">
         <f aca="false">F24*G24</f>
-        <v>194.4</v>
-      </c>
-      <c r="I24" s="3" t="n">
-        <f aca="false">F24*$C$11*0.0036*$C$10</f>
-        <v>2015.5392</v>
-      </c>
-      <c r="J24" s="9" t="n">
+        <v>76.464</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <f aca="false">F24*G24*$C$11*watthour_to_MJ</f>
+        <v>2413.0203264</v>
+      </c>
+      <c r="J24" s="10" t="n">
         <f aca="false">I24/($C$12*1000)</f>
-        <v>0.0248595405086811</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+        <v>0.0265392562032406</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="5" t="n">
         <f aca="false">1/D25</f>
         <v>10</v>
       </c>
-      <c r="D25" s="7" t="n">
+      <c r="D25" s="8" t="n">
         <v>0.1</v>
       </c>
-      <c r="E25" s="8" t="n">
+      <c r="E25" s="9" t="n">
         <v>58.3</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="5" t="n">
         <f aca="false">D25*E25</f>
         <v>5.83</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H25" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H25" s="4" t="n">
         <f aca="false">F25*G25</f>
-        <v>174.9</v>
-      </c>
-      <c r="I25" s="3" t="n">
-        <f aca="false">F25*$C$11*0.0036*$C$10</f>
-        <v>1813.3632</v>
-      </c>
-      <c r="J25" s="9" t="n">
+        <v>68.794</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <f aca="false">F25*G25*$C$11*watthour_to_MJ</f>
+        <v>2170.9735344</v>
+      </c>
+      <c r="J25" s="10" t="n">
         <f aca="false">I25/($C$12*1000)</f>
-        <v>0.0223659137601252</v>
-      </c>
-      <c r="K25" s="3"/>
+        <v>0.0238771394544587</v>
+      </c>
+      <c r="K25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="8" t="n">
         <v>5.32</v>
       </c>
-      <c r="D26" s="4" t="n">
+      <c r="D26" s="5" t="n">
         <f aca="false">1/C26</f>
         <v>0.18796992481203</v>
       </c>
-      <c r="E26" s="8" t="n">
+      <c r="E26" s="9" t="n">
         <v>28.3</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="5" t="n">
         <f aca="false">D26*E26</f>
         <v>5.31954887218045</v>
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H26" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H26" s="4" t="n">
         <f aca="false">F26*G26</f>
-        <v>159.586466165414</v>
-      </c>
-      <c r="I26" s="3" t="n">
-        <f aca="false">F26*$C$11*0.0036*$C$10</f>
-        <v>1654.59248120301</v>
-      </c>
-      <c r="J26" s="9" t="n">
+        <v>62.7706766917293</v>
+      </c>
+      <c r="I26" s="4" t="n">
+        <f aca="false">F26*G26*$C$11*watthour_to_MJ</f>
+        <v>1980.89190676692</v>
+      </c>
+      <c r="J26" s="10" t="n">
         <f aca="false">I26/($C$12*1000)</f>
-        <v>0.0204076451660307</v>
-      </c>
-      <c r="K26" s="3"/>
+        <v>0.0217865540747618</v>
+      </c>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="8" t="n">
         <v>2.95</v>
       </c>
-      <c r="D27" s="4" t="n">
+      <c r="D27" s="5" t="n">
         <f aca="false">1/C27</f>
         <v>0.338983050847458</v>
       </c>
-      <c r="E27" s="8" t="n">
+      <c r="E27" s="9" t="n">
         <v>11.5</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="5" t="n">
         <f aca="false">D27*E27</f>
         <v>3.89830508474576</v>
       </c>
       <c r="G27" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H27" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H27" s="4" t="n">
         <f aca="false">F27*G27</f>
-        <v>116.949152542373</v>
-      </c>
-      <c r="I27" s="3" t="n">
-        <f aca="false">F27*$C$11*0.0036*$C$10</f>
-        <v>1212.52881355932</v>
-      </c>
-      <c r="J27" s="9" t="n">
+        <v>46</v>
+      </c>
+      <c r="I27" s="4" t="n">
+        <f aca="false">F27*G27*$C$11*watthour_to_MJ</f>
+        <v>1451.6496</v>
+      </c>
+      <c r="J27" s="10" t="n">
         <f aca="false">I27/($C$12*1000)</f>
-        <v>0.0149552582051597</v>
-      </c>
-      <c r="K27" s="3"/>
+        <v>0.0159657588584048</v>
+      </c>
+      <c r="K27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="8" t="n">
         <v>2.51</v>
       </c>
-      <c r="D28" s="4" t="n">
+      <c r="D28" s="5" t="n">
         <f aca="false">1/C28</f>
         <v>0.398406374501992</v>
       </c>
-      <c r="E28" s="8" t="n">
+      <c r="E28" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="5" t="n">
         <f aca="false">D28*E28</f>
         <v>3.58565737051793</v>
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H28" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H28" s="4" t="n">
         <f aca="false">F28*G28</f>
-        <v>107.569721115538</v>
-      </c>
-      <c r="I28" s="3" t="n">
-        <f aca="false">F28*$C$11*0.0036*$C$10</f>
-        <v>1115.2828685259</v>
-      </c>
-      <c r="J28" s="9" t="n">
+        <v>42.3107569721116</v>
+      </c>
+      <c r="I28" s="4" t="n">
+        <f aca="false">F28*G28*$C$11*watthour_to_MJ</f>
+        <v>1335.22594422311</v>
+      </c>
+      <c r="J28" s="10" t="n">
         <f aca="false">I28/($C$12*1000)</f>
-        <v>0.0137558325081237</v>
-      </c>
-      <c r="K28" s="3"/>
+        <v>0.0146852900637675</v>
+      </c>
+      <c r="K28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="8" t="n">
         <v>5.3</v>
       </c>
-      <c r="D29" s="4" t="n">
+      <c r="D29" s="5" t="n">
         <f aca="false">1/C29</f>
         <v>0.188679245283019</v>
       </c>
-      <c r="E29" s="8" t="n">
+      <c r="E29" s="9" t="n">
         <v>8.7</v>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="5" t="n">
         <f aca="false">D29*E29</f>
         <v>1.64150943396226</v>
       </c>
       <c r="G29" s="0" t="n">
         <f aca="false">$B$5-$B$4</f>
-        <v>30</v>
-      </c>
-      <c r="H29" s="3" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="H29" s="4" t="n">
         <f aca="false">F29*G29</f>
-        <v>49.2452830188679</v>
-      </c>
-      <c r="I29" s="3" t="n">
-        <f aca="false">F29*$C$11*0.0036*$C$10</f>
-        <v>510.575094339623</v>
-      </c>
-      <c r="J29" s="9" t="n">
+        <v>19.3698113207547</v>
+      </c>
+      <c r="I29" s="4" t="n">
+        <f aca="false">F29*G29*$C$11*watthour_to_MJ</f>
+        <v>611.264757735849</v>
+      </c>
+      <c r="J29" s="10" t="n">
         <f aca="false">I29/($C$12*1000)</f>
-        <v>0.00629740281928506</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>38</v>
+        <v>0.00672290731912978</v>
+      </c>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="5"/>
+      <c r="H30" s="4" t="n">
+        <f aca="false">B38</f>
+        <v>3.28573050039337</v>
+      </c>
+      <c r="I30" s="4" t="n">
+        <f aca="false">H30*$C$11*watthour_to_MJ</f>
+        <v>103.689768839214</v>
+      </c>
+      <c r="J30" s="10" t="n">
+        <f aca="false">I30/($C$12*1000)</f>
+        <v>0.00114041697484753</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="3" t="n">
-        <f aca="false">B35*60/B33*(0.3048^3)</f>
-        <v>626.013915428572</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="A32" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1596,65 +1834,104 @@
       <c r="A33" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>1.75</v>
+      <c r="B33" s="4" t="n">
+        <f aca="false">B36*60/B34*(0.3048^3)</f>
+        <v>626.013915428572</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="H33" s="11" t="s">
         <v>43</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>416</v>
+        <v>1.75</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0.7171</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B35" s="0" t="n">
-        <f aca="false">B34*10/(2.54^2)</f>
-        <v>644.801289602579</v>
+        <v>416</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <f aca="false">0.018*(9/5)*0.2930710702/(0.3048^3)</f>
-        <v>0.335330512302265</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>1.276</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B36" s="0" t="n">
-        <f aca="false">B5-B4</f>
-        <v>30</v>
-      </c>
+        <f aca="false">B35*10/(2.54^2)</f>
+        <v>644.801289602579</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">1/3600</f>
+        <v>0.000277777777777778</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="3" t="n">
-        <f aca="false">B32*B36*B33*I35</f>
-        <v>11020.882265873</v>
+        <v>56</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">B5-B4</f>
+        <v>11.8</v>
+      </c>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <f aca="false">H34*H35*B34*B33*B37*H36</f>
+        <v>3.28573050039337</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K33" r:id="rId1" display="https://www.engineeringtoolbox.com/heat-loss-buildings-d_113.html"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1662,7 +1939,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1673,8 +1950,8 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1696,15 +1973,15 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>65</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <f aca="false">(B2-32)*5/9</f>
         <v>18.3333333333333</v>
       </c>
@@ -1712,7 +1989,7 @@
         <v>8</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="N2" s="0" t="n">
         <f aca="false">0.3048^2</f>
@@ -1721,16 +1998,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <f aca="false">6</f>
         <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <f aca="false">(B3-32)*5/9</f>
         <v>-14.4444444444444</v>
       </c>
@@ -1738,52 +2015,52 @@
         <v>8</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>0.1761</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <f aca="false">SUM(H15:H28)</f>
         <v>772.018768872121</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>3.412141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="3" t="n">
+      <c r="A6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="4" t="n">
         <f aca="false">B5*BTU_per_wh</f>
         <v>2634.23689403809</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="2" t="n">
         <v>3600</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -1791,11 +2068,11 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="5" t="n">
         <f aca="false">24*C8/C10</f>
         <v>9.85626283367557</v>
       </c>
@@ -1804,370 +2081,952 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">24*365.25</f>
         <v>8766</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9" t="n">
         <f aca="false">SUM(I15:I28)/1000</f>
         <v>16.0085811913323</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="5" t="n">
         <f aca="false">1000*C11/C8</f>
         <v>4.44682810870342</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="3" t="n">
+      <c r="H13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="4" t="n">
         <f aca="false">SUM(I15:I28)</f>
         <v>16008.5811913323</v>
       </c>
-      <c r="M13" s="3"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="F14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="12" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="C15" s="4" t="n">
+      <c r="C15" s="5" t="n">
         <f aca="false">B15*RSI_per_R</f>
         <v>2.2893</v>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D15" s="5" t="n">
         <f aca="false">1/C15</f>
         <v>0.436814746865854</v>
       </c>
-      <c r="E15" s="8" t="n">
+      <c r="E15" s="9" t="n">
         <f aca="false">((2*26+20)*8)*M2_per_sqft</f>
         <v>53.51215104</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <f aca="false">D15*E15</f>
         <v>23.374896710785</v>
       </c>
-      <c r="G15" s="3" t="n">
+      <c r="G15" s="4" t="n">
         <f aca="false">(($B$2-$B$3)-32)*5/9</f>
         <v>15</v>
       </c>
-      <c r="H15" s="3" t="n">
+      <c r="H15" s="4" t="n">
         <f aca="false">F15*G15</f>
         <v>350.623450661774</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="4" t="n">
         <f aca="false">F15*$C$10*0.0036*$C$9</f>
         <v>7270.52787292256</v>
       </c>
-      <c r="J15" s="9" t="n">
+      <c r="J15" s="10" t="n">
         <f aca="false">I15/$I$13</f>
         <v>0.45416441257512</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="12" t="n">
+        <v>71</v>
+      </c>
+      <c r="B16" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="C16" s="4" t="n">
+      <c r="C16" s="5" t="n">
         <f aca="false">B16*RSI_per_R</f>
         <v>3.3459</v>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="5" t="n">
         <f aca="false">1/C16</f>
         <v>0.298873247855584</v>
       </c>
-      <c r="E16" s="8" t="n">
+      <c r="E16" s="9" t="n">
         <f aca="false">520*M2_per_sqft</f>
         <v>48.3095808</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <f aca="false">D16*E16</f>
         <v>14.4384413162378</v>
       </c>
-      <c r="G16" s="3" t="n">
+      <c r="G16" s="4" t="n">
         <f aca="false">(($B$2-$B$3)-32)*5/9</f>
         <v>15</v>
       </c>
-      <c r="H16" s="3" t="n">
+      <c r="H16" s="4" t="n">
         <f aca="false">F16*G16</f>
         <v>216.576619743567</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <f aca="false">F16*$C$10*0.0036*$C$9</f>
         <v>4490.9327870026</v>
       </c>
-      <c r="J16" s="9" t="n">
+      <c r="J16" s="10" t="n">
         <f aca="false">I16/$I$13</f>
         <v>0.280532842562848</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="12" t="n">
+        <v>72</v>
+      </c>
+      <c r="B17" s="15" t="n">
         <v>7.5</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="C17" s="5" t="n">
         <f aca="false">B17*RSI_per_R</f>
         <v>1.32075</v>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="5" t="n">
         <f aca="false">1/C17</f>
         <v>0.757145561234147</v>
       </c>
-      <c r="E17" s="8" t="n">
+      <c r="E17" s="9" t="n">
         <f aca="false">20*8*M2_per_sqft</f>
         <v>14.8644864</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <f aca="false">D17*E17</f>
         <v>11.2545798977854</v>
       </c>
-      <c r="G17" s="3" t="n">
+      <c r="G17" s="4" t="n">
         <f aca="false">(($B$2-$B$3)-32)*5/9</f>
         <v>15</v>
       </c>
-      <c r="H17" s="3" t="n">
+      <c r="H17" s="4" t="n">
         <f aca="false">F17*G17</f>
         <v>168.81869846678</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="4" t="n">
         <f aca="false">F17*$C$10*0.0036*$C$9</f>
         <v>3500.62453140716</v>
       </c>
-      <c r="J17" s="9" t="n">
+      <c r="J17" s="10" t="n">
         <f aca="false">I17/$I$13</f>
         <v>0.218671754202836</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="8" t="n">
+        <v>73</v>
+      </c>
+      <c r="B18" s="9" t="n">
         <f aca="false">C18/RSI_per_R</f>
         <v>1.89286390308537</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="C18" s="5" t="n">
         <f aca="false">1/D18</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="E18" s="8" t="n">
+      <c r="E18" s="9" t="n">
         <f aca="false">0.8</f>
         <v>0.8</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="5" t="n">
         <f aca="false">D18*E18</f>
         <v>2.4</v>
       </c>
-      <c r="G18" s="3" t="n">
+      <c r="G18" s="4" t="n">
         <f aca="false">(($B$2-$B$3)-32)*5/9</f>
         <v>15</v>
       </c>
-      <c r="H18" s="3" t="n">
+      <c r="H18" s="4" t="n">
         <f aca="false">F18*G18</f>
         <v>36</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="4" t="n">
         <f aca="false">F18*$C$10*0.0036*$C$9</f>
         <v>746.496</v>
       </c>
-      <c r="J18" s="9" t="n">
+      <c r="J18" s="10" t="n">
         <f aca="false">I18/$I$13</f>
-        <v>0.0466309906591962</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+        <v>0.0466309906591961</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="4"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="5"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="8"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="8"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="9"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="8"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="9"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="8"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="9"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="8"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="8"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="9"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="8"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="9"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="9"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="10"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.39"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <f aca="false">SUM(H16:H23)</f>
+        <v>5686.20697916709</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3600</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <f aca="false">24*C9/C11</f>
+        <v>9.85626283367557</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">24*365.25</f>
+        <v>8766</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <f aca="false">SUM(I16:I23)/1000</f>
+        <v>58.9545939600044</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="5" t="n">
+        <f aca="false">1000*C12/C9</f>
+        <v>16.3762761000012</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <f aca="false">1/D16</f>
+        <v>0.440528634361233</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="E16" s="9" t="n">
+        <v>34.65</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <f aca="false">D16*E16</f>
+        <v>78.6555</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <f aca="false">F16*G16</f>
+        <v>2359.665</v>
+      </c>
+      <c r="I16" s="4" t="n">
+        <f aca="false">F16*$C$11*0.0036*$C$10</f>
+        <v>24465.00672</v>
+      </c>
+      <c r="J16" s="10" t="n">
+        <f aca="false">I16/($C$12*1000)</f>
+        <v>0.414980497306069</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <f aca="false">1/C17</f>
+        <v>0.258397932816537</v>
+      </c>
+      <c r="E17" s="9" t="n">
+        <v>119.9</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <f aca="false">D17*E17</f>
+        <v>30.9819121447028</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <f aca="false">F17*G17</f>
+        <v>929.457364341085</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <f aca="false">F17*$C$11*0.0036*$C$10</f>
+        <v>9636.61395348837</v>
+      </c>
+      <c r="J17" s="10" t="n">
+        <f aca="false">I17/($C$12*1000)</f>
+        <v>0.163458236350945</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="16" t="n">
+        <f aca="false">(3+2*2.7+2*2.6+3*2.6+2.4+2.2+2.1*8+2*2+4*2+2)/25</f>
+        <v>2.272</v>
+      </c>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <f aca="false">1/C18</f>
+        <v>0.258397932816537</v>
+      </c>
+      <c r="E18" s="9" t="n">
+        <v>107.8</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <f aca="false">D18*E18</f>
+        <v>27.8552971576227</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <f aca="false">F18*G18</f>
+        <v>835.658914728682</v>
+      </c>
+      <c r="I18" s="4" t="n">
+        <f aca="false">F18*$C$11*0.0036*$C$10</f>
+        <v>8664.11162790698</v>
+      </c>
+      <c r="J18" s="10" t="n">
+        <f aca="false">I18/($C$12*1000)</f>
+        <v>0.146962451031124</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <f aca="false">1/C19</f>
+        <v>0.226757369614512</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <v>92.2</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <f aca="false">D19*E19</f>
+        <v>20.907029478458</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H19" s="4" t="n">
+        <f aca="false">F19*G19</f>
+        <v>627.210884353741</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <f aca="false">F19*$C$11*0.0036*$C$10</f>
+        <v>6502.92244897959</v>
+      </c>
+      <c r="J19" s="10" t="n">
+        <f aca="false">I19/($C$12*1000)</f>
+        <v>0.110303913777971</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <v>6.85</v>
+      </c>
+      <c r="D20" s="5" t="n">
+        <f aca="false">1/C20</f>
+        <v>0.145985401459854</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <v>96.9</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <f aca="false">D20*E20</f>
+        <v>14.1459854014599</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <f aca="false">F20*G20</f>
+        <v>424.379562043796</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <f aca="false">F20*$C$11*0.0036*$C$10</f>
+        <v>4399.96729927007</v>
+      </c>
+      <c r="J20" s="10" t="n">
+        <f aca="false">I20/($C$12*1000)</f>
+        <v>0.0746331541568257</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <f aca="false">1/D21</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9" t="n">
+        <v>8.08</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <f aca="false">D21*E21</f>
+        <v>8.08</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H21" s="4" t="n">
+        <f aca="false">F21*G21</f>
+        <v>242.4</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <f aca="false">F21*$C$11*0.0036*$C$10</f>
+        <v>2513.2032</v>
+      </c>
+      <c r="J21" s="10" t="n">
+        <f aca="false">I21/($C$12*1000)</f>
+        <v>0.0426294717881526</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="D22" s="5" t="n">
+        <f aca="false">1/C22</f>
+        <v>0.284090909090909</v>
+      </c>
+      <c r="E22" s="9" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <f aca="false">D22*E22</f>
+        <v>5.42613636363636</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <f aca="false">F22*G22</f>
+        <v>162.784090909091</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <f aca="false">F22*$C$11*0.0036*$C$10</f>
+        <v>1687.74545454545</v>
+      </c>
+      <c r="J22" s="10" t="n">
+        <f aca="false">I22/($C$12*1000)</f>
+        <v>0.0286278870089487</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="D23" s="5" t="n">
+        <f aca="false">1/C23</f>
+        <v>0.258397932816537</v>
+      </c>
+      <c r="E23" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <f aca="false">D23*E23</f>
+        <v>3.48837209302326</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">$B$5-$B$4</f>
+        <v>30</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <f aca="false">F23*G23</f>
+        <v>104.651162790698</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <f aca="false">F23*$C$11*0.0036*$C$10</f>
+        <v>1085.02325581395</v>
+      </c>
+      <c r="J23" s="10" t="n">
+        <f aca="false">I23/($C$12*1000)</f>
+        <v>0.0184043885799646</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="4" t="n">
+        <f aca="false">B29*60/B27*(0.3048^3)</f>
+        <v>745.358919344262</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>345.3</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="9" t="n">
+        <f aca="false">B28*10/(2.54^2)</f>
+        <v>535.216070432141</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">B5-B4</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="4" t="n">
+        <f aca="false">house!H34*house!H35*B26*B27*B30*house!H36</f>
+        <v>6.93384987238732</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>